<commit_message>
split create and sheet create
</commit_message>
<xml_diff>
--- a/testing_dir/Points List Template - Copy.xlsx
+++ b/testing_dir/Points List Template - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delta\PycharmProjects\Project Tracking Excel Sheet\testing_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1631E421-6BF9-421C-8F36-727ED64791FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA1108C-84B6-431E-BC03-27AC2518F091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="923" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4755" yWindow="2505" windowWidth="21600" windowHeight="11295" tabRatio="923" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAC-304 EF-6" sheetId="37" r:id="rId1"/>
@@ -112,9 +112,6 @@
     </r>
   </si>
   <si>
-    <t>[Site Name Here]</t>
-  </si>
-  <si>
     <t>fart joke here</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
   </si>
   <si>
     <t>Sfarfrpare</t>
+  </si>
+  <si>
+    <t>Site Name Here</t>
   </si>
 </sst>
 </file>
@@ -814,7 +814,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -830,7 +830,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -841,7 +841,7 @@
     </row>
     <row r="2" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -900,7 +900,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="4" t="s">
@@ -910,7 +910,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -921,7 +921,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="5" t="s">
@@ -931,7 +931,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>